<commit_message>
Fix issue missing CF for `Carbon dioxide, non-fossil`
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gwp2021_100a_w_bio.xlsx
+++ b/premise_gwp/data/lcia_gwp2021_100a_w_bio.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise_gwp/premise_gwp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A75A64-74F6-7C41-BDC6-1732470A3828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3522E88E-E7AD-594B-890E-378001703384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="1540" windowWidth="28800" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$255</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$260</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Carbon dioxide, non-fossil, resource correction</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, non-fossil</t>
   </si>
 </sst>
 </file>
@@ -603,9 +606,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C255"/>
+  <dimension ref="A1:C260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -711,12 +714,12 @@
         <v>66</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -727,7 +730,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
         <v>47</v>
@@ -738,7 +741,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
@@ -749,7 +752,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
@@ -760,7 +763,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
         <v>48</v>
@@ -771,10 +774,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -782,10 +785,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -793,10 +796,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -804,10 +807,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -815,10 +818,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -826,109 +829,109 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C20">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C22">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
         <v>49</v>
       </c>
       <c r="C24">
-        <v>4.0624000000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C25">
-        <v>4.0624000000000002</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C26">
-        <v>4.0624000000000002</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C27">
-        <v>4.0624000000000002</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C28">
-        <v>4.0624000000000002</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29">
         <v>4.0624000000000002</v>
@@ -936,10 +939,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30">
         <v>4.0624000000000002</v>
@@ -947,10 +950,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31">
         <v>4.0624000000000002</v>
@@ -958,10 +961,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32">
         <v>4.0624000000000002</v>
@@ -969,10 +972,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C33">
         <v>4.0624000000000002</v>
@@ -980,1660 +983,1660 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34">
-        <v>2.4910000000000001</v>
+        <v>4.0624000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35">
-        <v>2.4910000000000001</v>
+        <v>4.0624000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36">
-        <v>2.4910000000000001</v>
+        <v>4.0624000000000002</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C37">
-        <v>2.4910000000000001</v>
+        <v>4.0624000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C38">
-        <v>2.4910000000000001</v>
+        <v>4.0624000000000002</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
         <v>49</v>
       </c>
       <c r="C39">
-        <v>20.6</v>
+        <v>2.4910000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
         <v>47</v>
       </c>
       <c r="C40">
-        <v>20.6</v>
+        <v>2.4910000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
       </c>
       <c r="C41">
-        <v>20.6</v>
+        <v>2.4910000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
         <v>46</v>
       </c>
       <c r="C42">
-        <v>20.6</v>
+        <v>2.4910000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
       <c r="C43">
-        <v>20.6</v>
+        <v>2.4910000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
       </c>
       <c r="C44">
-        <v>273</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
       </c>
       <c r="C45">
-        <v>273</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
       </c>
       <c r="C46">
-        <v>273</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
       <c r="C47">
-        <v>273</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>
       </c>
       <c r="C48">
-        <v>273</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
       </c>
       <c r="C49">
-        <v>0.437</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
         <v>47</v>
       </c>
       <c r="C50">
-        <v>0.437</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
       <c r="C51">
-        <v>0.437</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
       </c>
       <c r="C52">
-        <v>0.437</v>
+        <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
         <v>48</v>
       </c>
       <c r="C53">
-        <v>0.437</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
         <v>49</v>
       </c>
       <c r="C54">
-        <v>2300</v>
+        <v>0.437</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
       </c>
       <c r="C55">
-        <v>2300</v>
+        <v>0.437</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
         <v>50</v>
       </c>
       <c r="C56">
-        <v>2300</v>
+        <v>0.437</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>46</v>
       </c>
       <c r="C57">
-        <v>2300</v>
+        <v>0.437</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>48</v>
       </c>
       <c r="C58">
-        <v>2300</v>
+        <v>0.437</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
         <v>49</v>
       </c>
       <c r="C59">
-        <v>860</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B60" t="s">
         <v>47</v>
       </c>
       <c r="C60">
-        <v>860</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
         <v>50</v>
       </c>
       <c r="C61">
-        <v>860</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B62" t="s">
         <v>46</v>
       </c>
       <c r="C62">
-        <v>860</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
         <v>48</v>
       </c>
       <c r="C63">
-        <v>860</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
         <v>49</v>
       </c>
       <c r="C64">
-        <v>164</v>
+        <v>860</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
         <v>47</v>
       </c>
       <c r="C65">
-        <v>164</v>
+        <v>860</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
         <v>50</v>
       </c>
       <c r="C66">
-        <v>164</v>
+        <v>860</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
         <v>46</v>
       </c>
       <c r="C67">
-        <v>164</v>
+        <v>860</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
         <v>48</v>
       </c>
       <c r="C68">
-        <v>164</v>
+        <v>860</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
         <v>49</v>
       </c>
       <c r="C69">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
         <v>47</v>
       </c>
       <c r="C70">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B71" t="s">
         <v>50</v>
       </c>
       <c r="C71">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
         <v>46</v>
       </c>
       <c r="C72">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
         <v>48</v>
       </c>
       <c r="C73">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B74" t="s">
         <v>49</v>
       </c>
       <c r="C74">
-        <v>5810</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
         <v>47</v>
       </c>
       <c r="C75">
-        <v>5810</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
         <v>50</v>
       </c>
       <c r="C76">
-        <v>5810</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B77" t="s">
         <v>46</v>
       </c>
       <c r="C77">
-        <v>5810</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s">
         <v>48</v>
       </c>
       <c r="C78">
-        <v>5810</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B79" t="s">
         <v>49</v>
       </c>
       <c r="C79">
-        <v>1530</v>
+        <v>5810</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B80" t="s">
         <v>47</v>
       </c>
       <c r="C80">
-        <v>1530</v>
+        <v>5810</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B81" t="s">
         <v>50</v>
       </c>
       <c r="C81">
-        <v>1530</v>
+        <v>5810</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B82" t="s">
         <v>46</v>
       </c>
       <c r="C82">
-        <v>1530</v>
+        <v>5810</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B83" t="s">
         <v>48</v>
       </c>
       <c r="C83">
-        <v>1530</v>
+        <v>5810</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C84">
-        <v>6520</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C85">
-        <v>6520</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C86">
-        <v>6520</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B87" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C87">
-        <v>6520</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C88">
-        <v>6520</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B89" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C89">
-        <v>1.3</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B90" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C90">
-        <v>1.3</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B91" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C91">
-        <v>1.3</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C92">
-        <v>1.3</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B93" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C93">
-        <v>1.3</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C94">
-        <v>9430</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C95">
-        <v>9430</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B96" t="s">
         <v>50</v>
       </c>
       <c r="C96">
-        <v>9430</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B97" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C97">
-        <v>9430</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C98">
-        <v>9430</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C99">
-        <v>597</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C100">
-        <v>597</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B101" t="s">
         <v>50</v>
       </c>
       <c r="C101">
-        <v>597</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B102" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C102">
-        <v>597</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B103" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C103">
-        <v>597</v>
+        <v>9430</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B104" t="s">
         <v>49</v>
       </c>
       <c r="C104">
-        <v>90.4</v>
+        <v>597</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
         <v>47</v>
       </c>
       <c r="C105">
-        <v>90.4</v>
+        <v>597</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B106" t="s">
         <v>50</v>
       </c>
       <c r="C106">
-        <v>90.4</v>
+        <v>597</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B107" t="s">
         <v>46</v>
       </c>
       <c r="C107">
-        <v>90.4</v>
+        <v>597</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B108" t="s">
         <v>48</v>
       </c>
       <c r="C108">
-        <v>90.4</v>
+        <v>597</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B109" t="s">
         <v>49</v>
       </c>
       <c r="C109">
-        <v>9600</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B110" t="s">
         <v>47</v>
       </c>
       <c r="C110">
-        <v>9600</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B111" t="s">
         <v>50</v>
       </c>
       <c r="C111">
-        <v>9600</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B112" t="s">
         <v>46</v>
       </c>
       <c r="C112">
-        <v>9600</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B113" t="s">
         <v>48</v>
       </c>
       <c r="C113">
-        <v>9600</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B114" t="s">
         <v>49</v>
       </c>
       <c r="C114">
-        <v>12400</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B115" t="s">
         <v>47</v>
       </c>
       <c r="C115">
-        <v>12400</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B116" t="s">
         <v>50</v>
       </c>
       <c r="C116">
-        <v>12400</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B117" t="s">
         <v>46</v>
       </c>
       <c r="C117">
-        <v>12400</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B118" t="s">
         <v>48</v>
       </c>
       <c r="C118">
-        <v>12400</v>
+        <v>9600</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B119" t="s">
         <v>49</v>
       </c>
       <c r="C119">
-        <v>3740</v>
+        <v>12400</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B120" t="s">
         <v>47</v>
       </c>
       <c r="C120">
-        <v>3740</v>
+        <v>12400</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B121" t="s">
         <v>50</v>
       </c>
       <c r="C121">
-        <v>3740</v>
+        <v>12400</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B122" t="s">
         <v>46</v>
       </c>
       <c r="C122">
-        <v>3740</v>
+        <v>12400</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B123" t="s">
         <v>48</v>
       </c>
       <c r="C123">
-        <v>3740</v>
+        <v>12400</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B124" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C124">
-        <v>11</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B125" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C125">
-        <v>11</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B126" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C126">
-        <v>11</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B127" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C127">
-        <v>11</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="B128" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C128">
-        <v>11</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B129" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C129">
-        <v>2.4300000000000002</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B130" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C130">
-        <v>2.4300000000000002</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B131" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C131">
-        <v>2.4300000000000002</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B132" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C132">
-        <v>2.4300000000000002</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B133" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C133">
-        <v>2.4300000000000002</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B134" t="s">
         <v>49</v>
       </c>
       <c r="C134">
-        <v>1930</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B135" t="s">
         <v>47</v>
       </c>
       <c r="C135">
-        <v>1930</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B136" t="s">
         <v>50</v>
       </c>
       <c r="C136">
-        <v>1930</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B137" t="s">
         <v>46</v>
       </c>
       <c r="C137">
-        <v>1930</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B138" t="s">
         <v>48</v>
       </c>
       <c r="C138">
-        <v>1930</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B139" t="s">
         <v>49</v>
       </c>
       <c r="C139">
-        <v>7200</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B140" t="s">
         <v>47</v>
       </c>
       <c r="C140">
-        <v>7200</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B141" t="s">
         <v>50</v>
       </c>
       <c r="C141">
-        <v>7200</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B142" t="s">
         <v>46</v>
       </c>
       <c r="C142">
-        <v>7200</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B143" t="s">
         <v>48</v>
       </c>
       <c r="C143">
-        <v>7200</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B144" t="s">
         <v>49</v>
       </c>
       <c r="C144">
-        <v>79.400000000000006</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B145" t="s">
         <v>47</v>
       </c>
       <c r="C145">
-        <v>79.400000000000006</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B146" t="s">
         <v>50</v>
       </c>
       <c r="C146">
-        <v>79.400000000000006</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B147" t="s">
         <v>46</v>
       </c>
       <c r="C147">
-        <v>79.400000000000006</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B148" t="s">
         <v>48</v>
       </c>
       <c r="C148">
-        <v>79.400000000000006</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B149" t="s">
         <v>49</v>
       </c>
       <c r="C149">
-        <v>1960</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B150" t="s">
         <v>47</v>
       </c>
       <c r="C150">
-        <v>1960</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B151" t="s">
         <v>50</v>
       </c>
       <c r="C151">
-        <v>1960</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B152" t="s">
         <v>46</v>
       </c>
       <c r="C152">
-        <v>1960</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B153" t="s">
         <v>48</v>
       </c>
       <c r="C153">
-        <v>1960</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B154" t="s">
         <v>49</v>
       </c>
       <c r="C154">
-        <v>16200</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B155" t="s">
         <v>47</v>
       </c>
       <c r="C155">
-        <v>16200</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B156" t="s">
         <v>50</v>
       </c>
       <c r="C156">
-        <v>16200</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B157" t="s">
         <v>46</v>
       </c>
       <c r="C157">
-        <v>16200</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B158" t="s">
         <v>48</v>
       </c>
       <c r="C158">
-        <v>16200</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B159" t="s">
         <v>49</v>
       </c>
       <c r="C159">
-        <v>11.2</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B160" t="s">
         <v>47</v>
       </c>
       <c r="C160">
-        <v>11.2</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B161" t="s">
         <v>50</v>
       </c>
       <c r="C161">
-        <v>11.2</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B162" t="s">
         <v>46</v>
       </c>
       <c r="C162">
-        <v>11.2</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B163" t="s">
         <v>48</v>
       </c>
       <c r="C163">
-        <v>11.2</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B164" t="s">
         <v>49</v>
       </c>
       <c r="C164">
-        <v>12500</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B165" t="s">
         <v>47</v>
       </c>
       <c r="C165">
-        <v>12500</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B166" t="s">
         <v>50</v>
       </c>
       <c r="C166">
-        <v>12500</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B167" t="s">
         <v>46</v>
       </c>
       <c r="C167">
-        <v>12500</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B168" t="s">
         <v>48</v>
       </c>
       <c r="C168">
-        <v>12500</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B169" t="s">
         <v>49</v>
       </c>
       <c r="C169">
-        <v>160</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B170" t="s">
         <v>47</v>
       </c>
       <c r="C170">
-        <v>160</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B171" t="s">
         <v>50</v>
       </c>
       <c r="C171">
-        <v>160</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B172" t="s">
         <v>46</v>
       </c>
       <c r="C172">
-        <v>160</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B173" t="s">
         <v>48</v>
       </c>
       <c r="C173">
-        <v>160</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B174" t="s">
         <v>49</v>
       </c>
       <c r="C174">
-        <v>771</v>
+        <v>160</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B175" t="s">
         <v>47</v>
       </c>
       <c r="C175">
-        <v>771</v>
+        <v>160</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B176" t="s">
         <v>50</v>
       </c>
       <c r="C176">
-        <v>771</v>
+        <v>160</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B177" t="s">
         <v>46</v>
       </c>
       <c r="C177">
-        <v>771</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B178" t="s">
         <v>48</v>
       </c>
       <c r="C178">
-        <v>771</v>
+        <v>160</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B179" t="s">
         <v>49</v>
       </c>
       <c r="C179">
-        <v>29.8</v>
+        <v>771</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B180" t="s">
         <v>47</v>
       </c>
       <c r="C180">
-        <v>29.8</v>
+        <v>771</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B181" t="s">
         <v>50</v>
       </c>
       <c r="C181">
-        <v>29.8</v>
+        <v>771</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B182" t="s">
         <v>46</v>
       </c>
       <c r="C182">
-        <v>29.8</v>
+        <v>771</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B183" t="s">
         <v>48</v>
       </c>
       <c r="C183">
-        <v>29.8</v>
+        <v>771</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B184" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C184">
         <v>29.8</v>
@@ -2641,10 +2644,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B185" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C185">
         <v>29.8</v>
@@ -2652,10 +2655,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B186" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C186">
         <v>29.8</v>
@@ -2663,10 +2666,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B187" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C187">
         <v>29.8</v>
@@ -2674,10 +2677,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B188" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C188">
         <v>29.8</v>
@@ -2685,112 +2688,112 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B189" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C189">
-        <v>5.54</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B190" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C190">
-        <v>5.54</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B191" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C191">
-        <v>5.54</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B192" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C192">
-        <v>5.54</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B193" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C193">
-        <v>5.54</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B194" t="s">
         <v>49</v>
       </c>
       <c r="C194">
-        <v>27</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B195" t="s">
         <v>47</v>
       </c>
       <c r="C195">
-        <v>29.8</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B196" t="s">
         <v>50</v>
       </c>
       <c r="C196">
-        <v>29.8</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B197" t="s">
         <v>46</v>
       </c>
       <c r="C197">
-        <v>29.8</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B198" t="s">
         <v>48</v>
       </c>
       <c r="C198">
-        <v>29.8</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
@@ -2798,7 +2801,7 @@
         <v>37</v>
       </c>
       <c r="B199" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C199">
         <v>27</v>
@@ -2809,10 +2812,10 @@
         <v>37</v>
       </c>
       <c r="B200" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C200">
-        <v>27</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
@@ -2820,10 +2823,10 @@
         <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C201">
-        <v>27</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
@@ -2831,599 +2834,654 @@
         <v>37</v>
       </c>
       <c r="B202" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C202">
-        <v>27</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B203" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C203">
-        <v>2200</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B204" t="s">
         <v>47</v>
       </c>
       <c r="C204">
-        <v>2200</v>
+        <v>27</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B205" t="s">
         <v>50</v>
       </c>
       <c r="C205">
-        <v>2200</v>
+        <v>27</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B206" t="s">
         <v>46</v>
       </c>
       <c r="C206">
-        <v>2200</v>
+        <v>27</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B207" t="s">
         <v>48</v>
       </c>
       <c r="C207">
-        <v>2200</v>
+        <v>27</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B208" t="s">
         <v>49</v>
       </c>
       <c r="C208">
-        <v>7380</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B209" t="s">
         <v>47</v>
       </c>
       <c r="C209">
-        <v>7380</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B210" t="s">
         <v>50</v>
       </c>
       <c r="C210">
-        <v>7380</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B211" t="s">
         <v>46</v>
       </c>
       <c r="C211">
-        <v>7380</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B212" t="s">
         <v>48</v>
       </c>
       <c r="C212">
-        <v>7380</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B213" t="s">
         <v>49</v>
       </c>
       <c r="C213">
-        <v>6230</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B214" t="s">
         <v>47</v>
       </c>
       <c r="C214">
-        <v>6230</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B215" t="s">
         <v>50</v>
       </c>
       <c r="C215">
-        <v>6230</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B216" t="s">
         <v>46</v>
       </c>
       <c r="C216">
-        <v>6230</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B217" t="s">
         <v>48</v>
       </c>
       <c r="C217">
-        <v>6230</v>
+        <v>7380</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B218" t="s">
         <v>49</v>
       </c>
       <c r="C218">
-        <v>14600</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B219" t="s">
         <v>47</v>
       </c>
       <c r="C219">
-        <v>14600</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B220" t="s">
         <v>50</v>
       </c>
       <c r="C220">
-        <v>14600</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B221" t="s">
         <v>46</v>
       </c>
       <c r="C221">
-        <v>14600</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B222" t="s">
         <v>48</v>
       </c>
       <c r="C222">
-        <v>14600</v>
+        <v>6230</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B223" t="s">
         <v>49</v>
       </c>
       <c r="C223">
-        <v>0.48099999999999998</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B224" t="s">
         <v>47</v>
       </c>
       <c r="C224">
-        <v>0.48099999999999998</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B225" t="s">
         <v>50</v>
       </c>
       <c r="C225">
-        <v>0.48099999999999998</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B226" t="s">
         <v>46</v>
       </c>
       <c r="C226">
-        <v>0.48099999999999998</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B227" t="s">
         <v>48</v>
       </c>
       <c r="C227">
-        <v>0.48099999999999998</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B228" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C228">
-        <v>-10.8</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B229" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C229">
-        <v>17400</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B230" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C230">
-        <v>17400</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B231" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C231">
-        <v>17400</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B232" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C232">
-        <v>17400</v>
+        <v>0.48099999999999998</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B233" t="s">
         <v>48</v>
       </c>
       <c r="C233">
-        <v>17400</v>
+        <v>-10.8</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B234" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C234">
-        <v>9220</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B235" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C235">
-        <v>0.02</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B236" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C236">
-        <v>0.02</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B237" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C237">
-        <v>0.02</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="B238" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C238">
-        <v>0.02</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B239" t="s">
         <v>48</v>
       </c>
       <c r="C239">
-        <v>0.02</v>
+        <v>9220</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B240" t="s">
         <v>49</v>
       </c>
       <c r="C240">
-        <v>25200</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B241" t="s">
         <v>47</v>
       </c>
       <c r="C241">
-        <v>25200</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B242" t="s">
         <v>50</v>
       </c>
       <c r="C242">
-        <v>25200</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B243" t="s">
         <v>46</v>
       </c>
       <c r="C243">
-        <v>25200</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B244" t="s">
         <v>48</v>
       </c>
       <c r="C244">
-        <v>25200</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B245" t="s">
         <v>49</v>
       </c>
       <c r="C245">
-        <v>6.34</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B246" t="s">
         <v>47</v>
       </c>
       <c r="C246">
-        <v>6.34</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B247" t="s">
         <v>50</v>
       </c>
       <c r="C247">
-        <v>6.34</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B248" t="s">
         <v>46</v>
       </c>
       <c r="C248">
-        <v>6.34</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B249" t="s">
         <v>48</v>
       </c>
       <c r="C249">
-        <v>6.34</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B250" t="s">
         <v>49</v>
       </c>
       <c r="C250">
-        <v>4.3999999999999997E-2</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B251" t="s">
         <v>47</v>
       </c>
       <c r="C251">
-        <v>4.3999999999999997E-2</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B252" t="s">
         <v>50</v>
       </c>
       <c r="C252">
-        <v>4.3999999999999997E-2</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B253" t="s">
         <v>46</v>
       </c>
       <c r="C253">
-        <v>4.3999999999999997E-2</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B254" t="s">
         <v>48</v>
       </c>
       <c r="C254">
-        <v>4.3999999999999997E-2</v>
+        <v>6.34</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
+        <v>59</v>
+      </c>
+      <c r="B255" t="s">
+        <v>49</v>
+      </c>
+      <c r="C255">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>59</v>
+      </c>
+      <c r="B256" t="s">
+        <v>47</v>
+      </c>
+      <c r="C256">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>59</v>
+      </c>
+      <c r="B257" t="s">
+        <v>50</v>
+      </c>
+      <c r="C257">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>59</v>
+      </c>
+      <c r="B258" t="s">
+        <v>46</v>
+      </c>
+      <c r="C258">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>59</v>
+      </c>
+      <c r="B259" t="s">
+        <v>48</v>
+      </c>
+      <c r="C259">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
         <v>64</v>
       </c>
-      <c r="B255" t="s">
-        <v>48</v>
-      </c>
-      <c r="C255">
+      <c r="B260" t="s">
+        <v>48</v>
+      </c>
+      <c r="C260">
         <v>4.5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C255" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C255">
-      <sortCondition ref="A1:A946"/>
+  <autoFilter ref="A1:C260" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C260">
+      <sortCondition ref="A1:A951"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix sign for "Carbon dioxide, resource correction" for GWP100 2021.
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gwp2021_100a_w_bio.xlsx
+++ b/premise_gwp/data/lcia_gwp2021_100a_w_bio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise_gwp/premise_gwp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3522E88E-E7AD-594B-890E-378001703384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1251A6CC-8A45-D04A-B6A0-0A777A34E0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="1540" windowWidth="28800" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <dimension ref="A1:C260"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +714,7 @@
         <v>66</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>